<commit_message>
adapt specs to mediscam vars
</commit_message>
<xml_diff>
--- a/mediscam_lookup.xlsx
+++ b/mediscam_lookup.xlsx
@@ -2020,7 +2020,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G87"/>
+  <dimension ref="A1:G86"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="B2" xSplit="1" ySplit="1" activePane="bottomRight" state="frozen"/>
@@ -2854,23 +2854,35 @@
       </c>
     </row>
     <row r="40" ht="20.05" customHeight="1">
-      <c r="A40" s="8"/>
-      <c r="B40" s="9"/>
-      <c r="C40" s="10"/>
-      <c r="D40" s="10"/>
+      <c r="A40" t="s" s="8">
+        <v>74</v>
+      </c>
+      <c r="B40" t="s" s="9">
+        <v>34</v>
+      </c>
+      <c r="C40" t="s" s="10">
+        <v>10</v>
+      </c>
+      <c r="D40" t="s" s="10">
+        <v>9</v>
+      </c>
       <c r="E40" s="11"/>
-      <c r="F40" s="11"/>
-      <c r="G40" s="11"/>
+      <c r="F40" s="12">
+        <v>10</v>
+      </c>
+      <c r="G40" s="12">
+        <v>1</v>
+      </c>
     </row>
     <row r="41" ht="20.05" customHeight="1">
       <c r="A41" t="s" s="8">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B41" t="s" s="9">
         <v>34</v>
       </c>
       <c r="C41" t="s" s="10">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D41" t="s" s="10">
         <v>9</v>
@@ -2885,13 +2897,13 @@
     </row>
     <row r="42" ht="20.05" customHeight="1">
       <c r="A42" t="s" s="8">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B42" t="s" s="9">
         <v>34</v>
       </c>
       <c r="C42" t="s" s="10">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D42" t="s" s="10">
         <v>9</v>
@@ -2906,34 +2918,34 @@
     </row>
     <row r="43" ht="20.05" customHeight="1">
       <c r="A43" t="s" s="8">
-        <v>76</v>
+        <v>7</v>
       </c>
       <c r="B43" t="s" s="9">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="C43" t="s" s="10">
-        <v>12</v>
+        <v>77</v>
       </c>
       <c r="D43" t="s" s="10">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E43" s="11"/>
       <c r="F43" s="12">
-        <v>10</v>
+        <v>96</v>
       </c>
       <c r="G43" s="12">
         <v>1</v>
       </c>
     </row>
-    <row r="44" ht="20.05" customHeight="1">
+    <row r="44" ht="32.05" customHeight="1">
       <c r="A44" t="s" s="8">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B44" t="s" s="9">
         <v>8</v>
       </c>
       <c r="C44" t="s" s="10">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D44" t="s" s="10">
         <v>10</v>
@@ -2948,13 +2960,13 @@
     </row>
     <row r="45" ht="32.05" customHeight="1">
       <c r="A45" t="s" s="8">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B45" t="s" s="9">
         <v>8</v>
       </c>
       <c r="C45" t="s" s="10">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D45" t="s" s="10">
         <v>10</v>
@@ -2969,13 +2981,13 @@
     </row>
     <row r="46" ht="32.05" customHeight="1">
       <c r="A46" t="s" s="8">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B46" t="s" s="9">
         <v>8</v>
       </c>
       <c r="C46" t="s" s="10">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D46" t="s" s="10">
         <v>10</v>
@@ -2988,18 +3000,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" ht="32.05" customHeight="1">
+    <row r="47" ht="20.05" customHeight="1">
       <c r="A47" t="s" s="8">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B47" t="s" s="9">
         <v>8</v>
       </c>
       <c r="C47" t="s" s="10">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D47" t="s" s="10">
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="E47" s="11"/>
       <c r="F47" s="12">
@@ -3011,7 +3023,7 @@
     </row>
     <row r="48" ht="20.05" customHeight="1">
       <c r="A48" t="s" s="8">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B48" t="s" s="9">
         <v>8</v>
@@ -3020,7 +3032,7 @@
         <v>77</v>
       </c>
       <c r="D48" t="s" s="10">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="E48" s="11"/>
       <c r="F48" s="12">
@@ -3032,7 +3044,7 @@
     </row>
     <row r="49" ht="20.05" customHeight="1">
       <c r="A49" t="s" s="8">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B49" t="s" s="9">
         <v>8</v>
@@ -3041,7 +3053,7 @@
         <v>77</v>
       </c>
       <c r="D49" t="s" s="10">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E49" s="11"/>
       <c r="F49" s="12">
@@ -3051,18 +3063,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" ht="20.05" customHeight="1">
+    <row r="50" ht="32.05" customHeight="1">
       <c r="A50" t="s" s="8">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B50" t="s" s="9">
         <v>8</v>
       </c>
       <c r="C50" t="s" s="10">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="D50" t="s" s="10">
-        <v>82</v>
+        <v>10</v>
       </c>
       <c r="E50" s="11"/>
       <c r="F50" s="12">
@@ -3074,7 +3086,7 @@
     </row>
     <row r="51" ht="32.05" customHeight="1">
       <c r="A51" t="s" s="8">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B51" t="s" s="9">
         <v>8</v>
@@ -3083,7 +3095,7 @@
         <v>83</v>
       </c>
       <c r="D51" t="s" s="10">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E51" s="11"/>
       <c r="F51" s="12">
@@ -3093,18 +3105,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" ht="32.05" customHeight="1">
+    <row r="52" ht="44.05" customHeight="1">
       <c r="A52" t="s" s="8">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B52" t="s" s="9">
         <v>8</v>
       </c>
       <c r="C52" t="s" s="10">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D52" t="s" s="10">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E52" s="11"/>
       <c r="F52" s="12">
@@ -3114,18 +3126,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" ht="44.05" customHeight="1">
+    <row r="53" ht="32.05" customHeight="1">
       <c r="A53" t="s" s="8">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B53" t="s" s="9">
         <v>8</v>
       </c>
       <c r="C53" t="s" s="10">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D53" t="s" s="10">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="E53" s="11"/>
       <c r="F53" s="12">
@@ -3137,13 +3149,13 @@
     </row>
     <row r="54" ht="32.05" customHeight="1">
       <c r="A54" t="s" s="8">
-        <v>27</v>
+        <v>85</v>
       </c>
       <c r="B54" t="s" s="9">
         <v>8</v>
       </c>
       <c r="C54" t="s" s="10">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D54" t="s" s="10">
         <v>45</v>
@@ -3158,13 +3170,13 @@
     </row>
     <row r="55" ht="32.05" customHeight="1">
       <c r="A55" t="s" s="8">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B55" t="s" s="9">
         <v>8</v>
       </c>
       <c r="C55" t="s" s="10">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D55" t="s" s="10">
         <v>45</v>
@@ -3177,15 +3189,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" ht="32.05" customHeight="1">
+    <row r="56" ht="20.05" customHeight="1">
       <c r="A56" t="s" s="8">
-        <v>87</v>
+        <v>29</v>
       </c>
       <c r="B56" t="s" s="9">
         <v>8</v>
       </c>
       <c r="C56" t="s" s="10">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="D56" t="s" s="10">
         <v>45</v>
@@ -3198,15 +3210,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" ht="20.05" customHeight="1">
+    <row r="57" ht="32.05" customHeight="1">
       <c r="A57" t="s" s="8">
-        <v>29</v>
+        <v>89</v>
       </c>
       <c r="B57" t="s" s="9">
         <v>8</v>
       </c>
       <c r="C57" t="s" s="10">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="D57" t="s" s="10">
         <v>45</v>
@@ -3221,13 +3233,13 @@
     </row>
     <row r="58" ht="32.05" customHeight="1">
       <c r="A58" t="s" s="8">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B58" t="s" s="9">
         <v>8</v>
       </c>
       <c r="C58" t="s" s="10">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D58" t="s" s="10">
         <v>45</v>
@@ -3242,16 +3254,16 @@
     </row>
     <row r="59" ht="32.05" customHeight="1">
       <c r="A59" t="s" s="8">
-        <v>91</v>
+        <v>30</v>
       </c>
       <c r="B59" t="s" s="9">
         <v>8</v>
       </c>
       <c r="C59" t="s" s="10">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="D59" t="s" s="10">
-        <v>45</v>
+        <v>93</v>
       </c>
       <c r="E59" s="11"/>
       <c r="F59" s="12">
@@ -3263,13 +3275,13 @@
     </row>
     <row r="60" ht="32.05" customHeight="1">
       <c r="A60" t="s" s="8">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B60" t="s" s="9">
         <v>8</v>
       </c>
       <c r="C60" t="s" s="10">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D60" t="s" s="10">
         <v>93</v>
@@ -3282,18 +3294,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" ht="32.05" customHeight="1">
+    <row r="61" ht="20.05" customHeight="1">
       <c r="A61" t="s" s="8">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B61" t="s" s="9">
-        <v>8</v>
+        <v>94</v>
       </c>
       <c r="C61" t="s" s="10">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D61" t="s" s="10">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="E61" s="11"/>
       <c r="F61" s="12">
@@ -3305,7 +3317,7 @@
     </row>
     <row r="62" ht="20.05" customHeight="1">
       <c r="A62" t="s" s="8">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B62" t="s" s="9">
         <v>94</v>
@@ -3314,7 +3326,7 @@
         <v>77</v>
       </c>
       <c r="D62" t="s" s="10">
-        <v>73</v>
+        <v>9</v>
       </c>
       <c r="E62" s="11"/>
       <c r="F62" s="12">
@@ -3326,7 +3338,7 @@
     </row>
     <row r="63" ht="20.05" customHeight="1">
       <c r="A63" t="s" s="8">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B63" t="s" s="9">
         <v>94</v>
@@ -3335,7 +3347,7 @@
         <v>77</v>
       </c>
       <c r="D63" t="s" s="10">
-        <v>9</v>
+        <v>95</v>
       </c>
       <c r="E63" s="11"/>
       <c r="F63" s="12">
@@ -3347,7 +3359,7 @@
     </row>
     <row r="64" ht="20.05" customHeight="1">
       <c r="A64" t="s" s="8">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B64" t="s" s="9">
         <v>94</v>
@@ -3356,7 +3368,7 @@
         <v>77</v>
       </c>
       <c r="D64" t="s" s="10">
-        <v>95</v>
+        <v>71</v>
       </c>
       <c r="E64" s="11"/>
       <c r="F64" s="12">
@@ -3368,12 +3380,14 @@
     </row>
     <row r="65" ht="20.05" customHeight="1">
       <c r="A65" t="s" s="8">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B65" t="s" s="9">
         <v>94</v>
       </c>
-      <c r="C65" s="10"/>
+      <c r="C65" t="s" s="10">
+        <v>78</v>
+      </c>
       <c r="D65" t="s" s="10">
         <v>71</v>
       </c>
@@ -3387,14 +3401,16 @@
     </row>
     <row r="66" ht="20.05" customHeight="1">
       <c r="A66" t="s" s="8">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B66" t="s" s="9">
         <v>94</v>
       </c>
-      <c r="C66" s="10"/>
+      <c r="C66" t="s" s="10">
+        <v>77</v>
+      </c>
       <c r="D66" t="s" s="10">
-        <v>71</v>
+        <v>96</v>
       </c>
       <c r="E66" s="11"/>
       <c r="F66" s="12">
@@ -3406,7 +3422,7 @@
     </row>
     <row r="67" ht="20.05" customHeight="1">
       <c r="A67" t="s" s="8">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B67" t="s" s="9">
         <v>94</v>
@@ -3415,7 +3431,7 @@
         <v>77</v>
       </c>
       <c r="D67" t="s" s="10">
-        <v>96</v>
+        <v>35</v>
       </c>
       <c r="E67" s="11"/>
       <c r="F67" s="12">
@@ -3427,7 +3443,7 @@
     </row>
     <row r="68" ht="20.05" customHeight="1">
       <c r="A68" t="s" s="8">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B68" t="s" s="9">
         <v>94</v>
@@ -3436,7 +3452,7 @@
         <v>77</v>
       </c>
       <c r="D68" t="s" s="10">
-        <v>35</v>
+        <v>97</v>
       </c>
       <c r="E68" s="11"/>
       <c r="F68" s="12">
@@ -3448,13 +3464,13 @@
     </row>
     <row r="69" ht="20.05" customHeight="1">
       <c r="A69" t="s" s="8">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B69" t="s" s="9">
         <v>94</v>
       </c>
       <c r="C69" t="s" s="10">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D69" t="s" s="10">
         <v>97</v>
@@ -3467,18 +3483,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" ht="20.05" customHeight="1">
+    <row r="70" ht="32.05" customHeight="1">
       <c r="A70" t="s" s="8">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B70" t="s" s="9">
         <v>94</v>
       </c>
       <c r="C70" t="s" s="10">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D70" t="s" s="10">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E70" s="11"/>
       <c r="F70" s="12">
@@ -3490,13 +3506,13 @@
     </row>
     <row r="71" ht="32.05" customHeight="1">
       <c r="A71" t="s" s="8">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B71" t="s" s="9">
         <v>94</v>
       </c>
       <c r="C71" t="s" s="10">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D71" t="s" s="10">
         <v>98</v>
@@ -3509,18 +3525,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" ht="32.05" customHeight="1">
+    <row r="72" ht="20.05" customHeight="1">
       <c r="A72" t="s" s="8">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B72" t="s" s="9">
         <v>94</v>
       </c>
       <c r="C72" t="s" s="10">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D72" t="s" s="10">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E72" s="11"/>
       <c r="F72" s="12">
@@ -3532,7 +3548,7 @@
     </row>
     <row r="73" ht="20.05" customHeight="1">
       <c r="A73" t="s" s="8">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B73" t="s" s="9">
         <v>94</v>
@@ -3541,7 +3557,7 @@
         <v>77</v>
       </c>
       <c r="D73" t="s" s="10">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E73" s="11"/>
       <c r="F73" s="12">
@@ -3551,9 +3567,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" ht="20.05" customHeight="1">
+    <row r="74" ht="32.05" customHeight="1">
       <c r="A74" t="s" s="8">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B74" t="s" s="9">
         <v>94</v>
@@ -3562,7 +3578,7 @@
         <v>77</v>
       </c>
       <c r="D74" t="s" s="10">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E74" s="11"/>
       <c r="F74" s="12">
@@ -3574,7 +3590,7 @@
     </row>
     <row r="75" ht="32.05" customHeight="1">
       <c r="A75" t="s" s="8">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B75" t="s" s="9">
         <v>94</v>
@@ -3583,7 +3599,7 @@
         <v>77</v>
       </c>
       <c r="D75" t="s" s="10">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E75" s="11"/>
       <c r="F75" s="12">
@@ -3593,18 +3609,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" ht="32.05" customHeight="1">
+    <row r="76" ht="20.05" customHeight="1">
       <c r="A76" t="s" s="8">
-        <v>58</v>
+        <v>103</v>
       </c>
       <c r="B76" t="s" s="9">
-        <v>94</v>
+        <v>61</v>
       </c>
       <c r="C76" t="s" s="10">
         <v>77</v>
       </c>
       <c r="D76" t="s" s="10">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="E76" s="11"/>
       <c r="F76" s="12">
@@ -3616,7 +3632,7 @@
     </row>
     <row r="77" ht="20.05" customHeight="1">
       <c r="A77" t="s" s="8">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B77" t="s" s="9">
         <v>61</v>
@@ -3625,7 +3641,7 @@
         <v>77</v>
       </c>
       <c r="D77" t="s" s="10">
-        <v>71</v>
+        <v>105</v>
       </c>
       <c r="E77" s="11"/>
       <c r="F77" s="12">
@@ -3637,7 +3653,7 @@
     </row>
     <row r="78" ht="20.05" customHeight="1">
       <c r="A78" t="s" s="8">
-        <v>104</v>
+        <v>68</v>
       </c>
       <c r="B78" t="s" s="9">
         <v>61</v>
@@ -3646,7 +3662,7 @@
         <v>77</v>
       </c>
       <c r="D78" t="s" s="10">
-        <v>105</v>
+        <v>73</v>
       </c>
       <c r="E78" s="11"/>
       <c r="F78" s="12">
@@ -3658,7 +3674,7 @@
     </row>
     <row r="79" ht="20.05" customHeight="1">
       <c r="A79" t="s" s="8">
-        <v>68</v>
+        <v>106</v>
       </c>
       <c r="B79" t="s" s="9">
         <v>61</v>
@@ -3667,7 +3683,7 @@
         <v>77</v>
       </c>
       <c r="D79" t="s" s="10">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="E79" s="11"/>
       <c r="F79" s="12">
@@ -3679,7 +3695,7 @@
     </row>
     <row r="80" ht="20.05" customHeight="1">
       <c r="A80" t="s" s="8">
-        <v>106</v>
+        <v>70</v>
       </c>
       <c r="B80" t="s" s="9">
         <v>61</v>
@@ -3688,7 +3704,7 @@
         <v>77</v>
       </c>
       <c r="D80" t="s" s="10">
-        <v>96</v>
+        <v>40</v>
       </c>
       <c r="E80" s="11"/>
       <c r="F80" s="12">
@@ -3698,9 +3714,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" ht="20.05" customHeight="1">
+    <row r="81" ht="32.05" customHeight="1">
       <c r="A81" t="s" s="8">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B81" t="s" s="9">
         <v>61</v>
@@ -3709,7 +3725,7 @@
         <v>77</v>
       </c>
       <c r="D81" t="s" s="10">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E81" s="11"/>
       <c r="F81" s="12">
@@ -3721,7 +3737,7 @@
     </row>
     <row r="82" ht="32.05" customHeight="1">
       <c r="A82" t="s" s="8">
-        <v>72</v>
+        <v>107</v>
       </c>
       <c r="B82" t="s" s="9">
         <v>61</v>
@@ -3730,7 +3746,7 @@
         <v>77</v>
       </c>
       <c r="D82" t="s" s="10">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="E82" s="11"/>
       <c r="F82" s="12">
@@ -3742,7 +3758,7 @@
     </row>
     <row r="83" ht="32.05" customHeight="1">
       <c r="A83" t="s" s="8">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B83" t="s" s="9">
         <v>61</v>
@@ -3751,7 +3767,7 @@
         <v>77</v>
       </c>
       <c r="D83" t="s" s="10">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="E83" s="11"/>
       <c r="F83" s="12">
@@ -3761,18 +3777,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" ht="32.05" customHeight="1">
+    <row r="84" ht="20.05" customHeight="1">
       <c r="A84" t="s" s="8">
-        <v>108</v>
+        <v>74</v>
       </c>
       <c r="B84" t="s" s="9">
-        <v>61</v>
+        <v>94</v>
       </c>
       <c r="C84" t="s" s="10">
         <v>77</v>
       </c>
       <c r="D84" t="s" s="10">
-        <v>28</v>
+        <v>109</v>
       </c>
       <c r="E84" s="11"/>
       <c r="F84" s="12">
@@ -3784,13 +3800,13 @@
     </row>
     <row r="85" ht="20.05" customHeight="1">
       <c r="A85" t="s" s="8">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B85" t="s" s="9">
         <v>94</v>
       </c>
       <c r="C85" t="s" s="10">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D85" t="s" s="10">
         <v>109</v>
@@ -3805,13 +3821,13 @@
     </row>
     <row r="86" ht="20.05" customHeight="1">
       <c r="A86" t="s" s="8">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B86" t="s" s="9">
         <v>94</v>
       </c>
       <c r="C86" t="s" s="10">
-        <v>78</v>
+        <v>110</v>
       </c>
       <c r="D86" t="s" s="10">
         <v>109</v>
@@ -3821,27 +3837,6 @@
         <v>96</v>
       </c>
       <c r="G86" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" ht="20.05" customHeight="1">
-      <c r="A87" t="s" s="8">
-        <v>76</v>
-      </c>
-      <c r="B87" t="s" s="9">
-        <v>94</v>
-      </c>
-      <c r="C87" t="s" s="10">
-        <v>110</v>
-      </c>
-      <c r="D87" t="s" s="10">
-        <v>109</v>
-      </c>
-      <c r="E87" s="11"/>
-      <c r="F87" s="12">
-        <v>96</v>
-      </c>
-      <c r="G87" s="12">
         <v>1</v>
       </c>
     </row>
@@ -4147,7 +4142,9 @@
       <c r="A26" t="s" s="20">
         <v>42</v>
       </c>
-      <c r="B26" s="23"/>
+      <c r="B26" t="s" s="23">
+        <v>134</v>
+      </c>
       <c r="C26" t="s" s="24">
         <v>140</v>
       </c>
@@ -4156,7 +4153,9 @@
       <c r="A27" t="s" s="20">
         <v>44</v>
       </c>
-      <c r="B27" s="21"/>
+      <c r="B27" t="s" s="21">
+        <v>134</v>
+      </c>
       <c r="C27" t="s" s="22">
         <v>141</v>
       </c>
@@ -4165,7 +4164,9 @@
       <c r="A28" t="s" s="20">
         <v>46</v>
       </c>
-      <c r="B28" s="23"/>
+      <c r="B28" t="s" s="23">
+        <v>134</v>
+      </c>
       <c r="C28" t="s" s="24">
         <v>142</v>
       </c>
@@ -4174,7 +4175,9 @@
       <c r="A29" t="s" s="20">
         <v>48</v>
       </c>
-      <c r="B29" s="21"/>
+      <c r="B29" t="s" s="21">
+        <v>134</v>
+      </c>
       <c r="C29" t="s" s="22">
         <v>143</v>
       </c>
@@ -4183,7 +4186,9 @@
       <c r="A30" t="s" s="20">
         <v>49</v>
       </c>
-      <c r="B30" s="23"/>
+      <c r="B30" t="s" s="23">
+        <v>134</v>
+      </c>
       <c r="C30" t="s" s="24">
         <v>144</v>
       </c>

</xml_diff>